<commit_message>
update models columns names
</commit_message>
<xml_diff>
--- a/data/results/results_final.xlsx
+++ b/data/results/results_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoavz\GitHub\APPETITE\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB3C60D-6893-432F-B54E-03516070C08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73015420-857B-44EB-A799-3BDFD3326378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged_results" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="279">
   <si>
     <t>after size</t>
   </si>
@@ -876,9 +876,6 @@
   </si>
   <si>
     <t>סכום של average Fuzzy_Participation_Error_Confidence_STAT_BARINEL_Features wasted effort</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fuzzy_Participation_Error_Confidence_STAT_BARINEL_Features accuracy increase</t>
   </si>
 </sst>
 </file>
@@ -6156,7 +6153,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Fuzzy_Participation_Error_Confidence_STAT_BARINEL_Features accuracy increase</c:v>
+                  <c:v>סכום של average Fuzzy_Participation_Error_Confidence_STAT_BARINEL_Features accuracy increase</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -31781,7 +31778,7 @@
     <dataField name="סכום של average Fuzzy_Participation_Error_Confidence_STAT_BARINEL accuracy increase" fld="264" baseField="0" baseItem="0"/>
     <dataField name="סכום של average Fuzzy_Participation_Confidence_STAT_BARINEL_Features accuracy increase" fld="265" baseField="0" baseItem="0"/>
     <dataField name="סכום של average Fuzzy_Error_Confidence_STAT_BARINEL_Features accuracy increase" fld="266" baseField="0" baseItem="0"/>
-    <dataField name=" Fuzzy_Participation_Error_Confidence_STAT_BARINEL_Features accuracy increase" fld="267" baseField="0" baseItem="0"/>
+    <dataField name="סכום של average Fuzzy_Participation_Error_Confidence_STAT_BARINEL_Features accuracy increase" fld="267" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="198">
     <chartFormat chart="0" format="0" series="1">
@@ -34873,7 +34870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GS67"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -75423,7 +75420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BN5"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A26" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="BK1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="BN4" sqref="BN4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -75705,7 +75704,7 @@
         <v>272</v>
       </c>
       <c r="BN4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update results after more finished
</commit_message>
<xml_diff>
--- a/data/results/results_final.xlsx
+++ b/data/results/results_final.xlsx
@@ -16589,115 +16589,115 @@
         <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>5069</v>
+        <v>5702</v>
       </c>
       <c r="G10" t="n">
-        <v>280546.5456490873</v>
+        <v>317826.2813319067</v>
       </c>
       <c r="H10" t="n">
-        <v>-50655.09552903478</v>
+        <v>-56052.45235722861</v>
       </c>
       <c r="I10" t="n">
-        <v>57045.93142812786</v>
+        <v>65677.20896116752</v>
       </c>
       <c r="J10" t="n">
-        <v>71388.75892076807</v>
+        <v>74162.76773134076</v>
       </c>
       <c r="K10" t="n">
-        <v>81564</v>
+        <v>99023</v>
       </c>
       <c r="L10" t="n">
-        <v>1252.666666666667</v>
+        <v>1387.666666666667</v>
       </c>
       <c r="M10" t="n">
-        <v>80361.93613269267</v>
+        <v>85297.91263783217</v>
       </c>
       <c r="N10" t="n">
-        <v>90332</v>
+        <v>101524</v>
       </c>
       <c r="O10" t="n">
-        <v>1252.666666666667</v>
+        <v>1387.666666666667</v>
       </c>
       <c r="P10" t="n">
-        <v>10348.11542205268</v>
+        <v>10202.8878155916</v>
       </c>
       <c r="Q10" t="n">
-        <v>48094</v>
+        <v>55137</v>
       </c>
       <c r="R10" t="n">
-        <v>555.6666666666666</v>
+        <v>605.6666666666666</v>
       </c>
       <c r="S10" t="n">
-        <v>17261.00845196548</v>
+        <v>17985.38436973347</v>
       </c>
       <c r="T10" t="n">
-        <v>44079</v>
+        <v>51074</v>
       </c>
       <c r="U10" t="n">
-        <v>691</v>
+        <v>783</v>
       </c>
       <c r="V10" t="n">
-        <v>70726.66234439</v>
+        <v>74608.60067038119</v>
       </c>
       <c r="W10" t="n">
-        <v>36931</v>
+        <v>43019</v>
       </c>
       <c r="X10" t="n">
-        <v>1306.666666666667</v>
+        <v>1502.333333333333</v>
       </c>
       <c r="Y10" t="n">
-        <v>17261.00845196548</v>
+        <v>17985.38436973347</v>
       </c>
       <c r="Z10" t="n">
-        <v>44079</v>
+        <v>51074</v>
       </c>
       <c r="AA10" t="n">
-        <v>691</v>
+        <v>783</v>
       </c>
       <c r="AB10" t="n">
-        <v>17261.00845196548</v>
+        <v>17985.38436973347</v>
       </c>
       <c r="AC10" t="n">
-        <v>44079</v>
+        <v>51074</v>
       </c>
       <c r="AD10" t="n">
-        <v>691</v>
+        <v>783</v>
       </c>
       <c r="AE10" t="n">
-        <v>69357.84452434123</v>
+        <v>73490.29680040583</v>
       </c>
       <c r="AF10" t="n">
-        <v>31362</v>
+        <v>37059</v>
       </c>
       <c r="AG10" t="n">
-        <v>1212.333333333333</v>
+        <v>1399.666666666667</v>
       </c>
       <c r="AH10" t="n">
-        <v>66701.49485471702</v>
+        <v>71115.44492813846</v>
       </c>
       <c r="AI10" t="n">
-        <v>36871</v>
+        <v>42851</v>
       </c>
       <c r="AJ10" t="n">
-        <v>1226.666666666667</v>
+        <v>1422.333333333333</v>
       </c>
       <c r="AK10" t="n">
-        <v>17261.00845196548</v>
+        <v>17985.38436973347</v>
       </c>
       <c r="AL10" t="n">
-        <v>44079</v>
+        <v>51074</v>
       </c>
       <c r="AM10" t="n">
-        <v>691</v>
+        <v>783</v>
       </c>
       <c r="AN10" t="n">
-        <v>70533.34145695352</v>
+        <v>74945.96994447187</v>
       </c>
       <c r="AO10" t="n">
-        <v>30007</v>
+        <v>35612</v>
       </c>
       <c r="AP10" t="n">
-        <v>1256.333333333333</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="11">
@@ -17777,115 +17777,115 @@
         <v>2</v>
       </c>
       <c r="F19" t="n">
-        <v>5052</v>
+        <v>5703</v>
       </c>
       <c r="G19" t="n">
-        <v>277334.288165384</v>
+        <v>315630.5512446067</v>
       </c>
       <c r="H19" t="n">
-        <v>-33053.96119136489</v>
+        <v>-40600.44848583425</v>
       </c>
       <c r="I19" t="n">
-        <v>69381.12176820097</v>
+        <v>80276.18903277497</v>
       </c>
       <c r="J19" t="n">
-        <v>72601.59833739625</v>
+        <v>75486.35170062495</v>
       </c>
       <c r="K19" t="n">
-        <v>76540</v>
+        <v>94876</v>
       </c>
       <c r="L19" t="n">
-        <v>1253.333333333333</v>
+        <v>1382.333333333333</v>
       </c>
       <c r="M19" t="n">
-        <v>81344.34877910261</v>
+        <v>85708.32486280963</v>
       </c>
       <c r="N19" t="n">
-        <v>86862</v>
+        <v>97193</v>
       </c>
       <c r="O19" t="n">
-        <v>1253.333333333333</v>
+        <v>1382.333333333333</v>
       </c>
       <c r="P19" t="n">
-        <v>13102.22545983295</v>
+        <v>12796.24638658931</v>
       </c>
       <c r="Q19" t="n">
-        <v>47866</v>
+        <v>55433</v>
       </c>
       <c r="R19" t="n">
-        <v>569.3333333333333</v>
+        <v>620.3333333333333</v>
       </c>
       <c r="S19" t="n">
-        <v>19079.53261884964</v>
+        <v>19840.22021227266</v>
       </c>
       <c r="T19" t="n">
-        <v>42524</v>
+        <v>50215</v>
       </c>
       <c r="U19" t="n">
-        <v>742.3333333333333</v>
+        <v>830.6666666666666</v>
       </c>
       <c r="V19" t="n">
-        <v>71524.08866259349</v>
+        <v>77395.2396341929</v>
       </c>
       <c r="W19" t="n">
-        <v>38989</v>
+        <v>45370</v>
       </c>
       <c r="X19" t="n">
-        <v>1420</v>
+        <v>1637.666666666667</v>
       </c>
       <c r="Y19" t="n">
-        <v>19079.53261884964</v>
+        <v>19840.22021227266</v>
       </c>
       <c r="Z19" t="n">
-        <v>42524</v>
+        <v>50215</v>
       </c>
       <c r="AA19" t="n">
-        <v>742.3333333333333</v>
+        <v>830.6666666666666</v>
       </c>
       <c r="AB19" t="n">
-        <v>19079.53261884964</v>
+        <v>19840.22021227266</v>
       </c>
       <c r="AC19" t="n">
-        <v>42524</v>
+        <v>50215</v>
       </c>
       <c r="AD19" t="n">
-        <v>742.3333333333333</v>
+        <v>830.6666666666666</v>
       </c>
       <c r="AE19" t="n">
-        <v>67410.37636361395</v>
+        <v>71818.44811249287</v>
       </c>
       <c r="AF19" t="n">
-        <v>33703</v>
+        <v>39628</v>
       </c>
       <c r="AG19" t="n">
-        <v>1249.333333333333</v>
+        <v>1435</v>
       </c>
       <c r="AH19" t="n">
-        <v>67885.66995430592</v>
+        <v>73607.19461798306</v>
       </c>
       <c r="AI19" t="n">
-        <v>40132</v>
+        <v>46607</v>
       </c>
       <c r="AJ19" t="n">
-        <v>1376.666666666667</v>
+        <v>1588</v>
       </c>
       <c r="AK19" t="n">
-        <v>19079.53261884964</v>
+        <v>19840.22021227266</v>
       </c>
       <c r="AL19" t="n">
-        <v>42524</v>
+        <v>50215</v>
       </c>
       <c r="AM19" t="n">
-        <v>742.3333333333333</v>
+        <v>830.6666666666666</v>
       </c>
       <c r="AN19" t="n">
-        <v>67743.38800644956</v>
+        <v>72786.8857642971</v>
       </c>
       <c r="AO19" t="n">
-        <v>30488</v>
+        <v>36687</v>
       </c>
       <c r="AP19" t="n">
-        <v>1245</v>
+        <v>1445.666666666667</v>
       </c>
     </row>
     <row r="20">
@@ -18965,115 +18965,115 @@
         <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>5333</v>
+        <v>6138</v>
       </c>
       <c r="G28" t="n">
-        <v>295918.7376127233</v>
+        <v>345406.0441142712</v>
       </c>
       <c r="H28" t="n">
-        <v>12525.61238765539</v>
+        <v>25967.8724495749</v>
       </c>
       <c r="I28" t="n">
-        <v>88531.31724150042</v>
+        <v>100131.3172415004</v>
       </c>
       <c r="J28" t="n">
-        <v>73106.49897559277</v>
+        <v>77073.21724184664</v>
       </c>
       <c r="K28" t="n">
-        <v>79990</v>
+        <v>102621</v>
       </c>
       <c r="L28" t="n">
-        <v>1354</v>
+        <v>1532.333333333333</v>
       </c>
       <c r="M28" t="n">
-        <v>84351.6393929894</v>
+        <v>90612.6301050637</v>
       </c>
       <c r="N28" t="n">
-        <v>89836</v>
+        <v>101899</v>
       </c>
       <c r="O28" t="n">
-        <v>1354</v>
+        <v>1532.333333333333</v>
       </c>
       <c r="P28" t="n">
-        <v>13796.25866653019</v>
+        <v>14022.72925476548</v>
       </c>
       <c r="Q28" t="n">
-        <v>49300</v>
+        <v>59254</v>
       </c>
       <c r="R28" t="n">
-        <v>664</v>
+        <v>737</v>
       </c>
       <c r="S28" t="n">
-        <v>27021.7509904805</v>
+        <v>29367.41662515542</v>
       </c>
       <c r="T28" t="n">
-        <v>43177</v>
+        <v>51083</v>
       </c>
       <c r="U28" t="n">
-        <v>876.3333333333334</v>
+        <v>1020.666666666667</v>
       </c>
       <c r="V28" t="n">
-        <v>71935.96786598742</v>
+        <v>78728.69232419175</v>
       </c>
       <c r="W28" t="n">
-        <v>43280</v>
+        <v>52673</v>
       </c>
       <c r="X28" t="n">
-        <v>1255.333333333333</v>
+        <v>1513.666666666667</v>
       </c>
       <c r="Y28" t="n">
-        <v>27021.7509904805</v>
+        <v>29367.41662515542</v>
       </c>
       <c r="Z28" t="n">
-        <v>43177</v>
+        <v>51083</v>
       </c>
       <c r="AA28" t="n">
-        <v>876.3333333333334</v>
+        <v>1020.666666666667</v>
       </c>
       <c r="AB28" t="n">
-        <v>27021.7509904805</v>
+        <v>29367.41662515542</v>
       </c>
       <c r="AC28" t="n">
-        <v>43177</v>
+        <v>51083</v>
       </c>
       <c r="AD28" t="n">
-        <v>876.3333333333334</v>
+        <v>1020.666666666667</v>
       </c>
       <c r="AE28" t="n">
-        <v>67020.58081854091</v>
+        <v>74636.37029222513</v>
       </c>
       <c r="AF28" t="n">
-        <v>41597</v>
+        <v>51419</v>
       </c>
       <c r="AG28" t="n">
-        <v>1334.666666666667</v>
+        <v>1585.333333333333</v>
       </c>
       <c r="AH28" t="n">
-        <v>68752.35528145374</v>
+        <v>75496.93732479739</v>
       </c>
       <c r="AI28" t="n">
-        <v>44204</v>
+        <v>53757</v>
       </c>
       <c r="AJ28" t="n">
-        <v>1253.333333333333</v>
+        <v>1512</v>
       </c>
       <c r="AK28" t="n">
-        <v>27021.7509904805</v>
+        <v>29367.41662515542</v>
       </c>
       <c r="AL28" t="n">
-        <v>43177</v>
+        <v>51083</v>
       </c>
       <c r="AM28" t="n">
-        <v>876.3333333333334</v>
+        <v>1020.666666666667</v>
       </c>
       <c r="AN28" t="n">
-        <v>65437.10814764015</v>
+        <v>73176.27223432745</v>
       </c>
       <c r="AO28" t="n">
-        <v>37552</v>
+        <v>47799</v>
       </c>
       <c r="AP28" t="n">
-        <v>1282.666666666667</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="29">
@@ -20153,115 +20153,115 @@
         <v>2</v>
       </c>
       <c r="F37" t="n">
-        <v>5677</v>
+        <v>6443</v>
       </c>
       <c r="G37" t="n">
-        <v>322807.3522067272</v>
+        <v>368919.8722709327</v>
       </c>
       <c r="H37" t="n">
-        <v>17979.25299118091</v>
+        <v>28179.41350482457</v>
       </c>
       <c r="I37" t="n">
-        <v>86394.35572902452</v>
+        <v>101537.533899169</v>
       </c>
       <c r="J37" t="n">
-        <v>77793.22524000311</v>
+        <v>81695.15140372702</v>
       </c>
       <c r="K37" t="n">
-        <v>80798</v>
+        <v>101350</v>
       </c>
       <c r="L37" t="n">
-        <v>1454.333333333333</v>
+        <v>1619</v>
       </c>
       <c r="M37" t="n">
-        <v>84499.07365652538</v>
+        <v>90375.47815090739</v>
       </c>
       <c r="N37" t="n">
-        <v>91405</v>
+        <v>101916</v>
       </c>
       <c r="O37" t="n">
-        <v>1454.666666666667</v>
+        <v>1619.333333333333</v>
       </c>
       <c r="P37" t="n">
-        <v>18304.71447538552</v>
+        <v>18688.50259737589</v>
       </c>
       <c r="Q37" t="n">
-        <v>53291</v>
+        <v>63171</v>
       </c>
       <c r="R37" t="n">
-        <v>740.6666666666666</v>
+        <v>811.3333333333333</v>
       </c>
       <c r="S37" t="n">
-        <v>29936.76114358223</v>
+        <v>32292.45937793215</v>
       </c>
       <c r="T37" t="n">
-        <v>45657</v>
+        <v>53157</v>
       </c>
       <c r="U37" t="n">
-        <v>974</v>
+        <v>1107</v>
       </c>
       <c r="V37" t="n">
-        <v>58759.17599161463</v>
+        <v>64088.54998840435</v>
       </c>
       <c r="W37" t="n">
-        <v>44977</v>
+        <v>53901</v>
       </c>
       <c r="X37" t="n">
-        <v>1284.333333333333</v>
+        <v>1517.666666666667</v>
       </c>
       <c r="Y37" t="n">
-        <v>29936.76114358223</v>
+        <v>32292.45937793215</v>
       </c>
       <c r="Z37" t="n">
-        <v>45657</v>
+        <v>53157</v>
       </c>
       <c r="AA37" t="n">
-        <v>974</v>
+        <v>1107</v>
       </c>
       <c r="AB37" t="n">
-        <v>29936.76114358223</v>
+        <v>32292.45937793215</v>
       </c>
       <c r="AC37" t="n">
-        <v>45657</v>
+        <v>53157</v>
       </c>
       <c r="AD37" t="n">
-        <v>974</v>
+        <v>1107</v>
       </c>
       <c r="AE37" t="n">
-        <v>58702.19998760593</v>
+        <v>65334.78425726885</v>
       </c>
       <c r="AF37" t="n">
-        <v>47283</v>
+        <v>56633</v>
       </c>
       <c r="AG37" t="n">
-        <v>1357</v>
+        <v>1582.333333333333</v>
       </c>
       <c r="AH37" t="n">
-        <v>56524.63255438714</v>
+        <v>61712.91505839997</v>
       </c>
       <c r="AI37" t="n">
-        <v>52077</v>
+        <v>61300</v>
       </c>
       <c r="AJ37" t="n">
-        <v>1301.333333333333</v>
+        <v>1533.666666666666</v>
       </c>
       <c r="AK37" t="n">
-        <v>29936.76114358223</v>
+        <v>32292.45937793215</v>
       </c>
       <c r="AL37" t="n">
-        <v>45657</v>
+        <v>53157</v>
       </c>
       <c r="AM37" t="n">
-        <v>974</v>
+        <v>1107</v>
       </c>
       <c r="AN37" t="n">
-        <v>58207.20515079661</v>
+        <v>64805.60001436001</v>
       </c>
       <c r="AO37" t="n">
-        <v>45922</v>
+        <v>55651</v>
       </c>
       <c r="AP37" t="n">
-        <v>1314</v>
+        <v>1540.333333333333</v>
       </c>
     </row>
     <row r="38">
@@ -21341,115 +21341,115 @@
         <v>2</v>
       </c>
       <c r="F46" t="n">
-        <v>5855</v>
+        <v>6639</v>
       </c>
       <c r="G46" t="n">
-        <v>336869.8609866071</v>
+        <v>384317.5276532738</v>
       </c>
       <c r="H46" t="n">
-        <v>25372.76636652031</v>
+        <v>39991.76636652031</v>
       </c>
       <c r="I46" t="n">
-        <v>101688.9134819897</v>
+        <v>119322.246815323</v>
       </c>
       <c r="J46" t="n">
-        <v>70759.72911135745</v>
+        <v>73885.06244469078</v>
       </c>
       <c r="K46" t="n">
-        <v>87017</v>
+        <v>107365</v>
       </c>
       <c r="L46" t="n">
-        <v>1397.333333333333</v>
+        <v>1557.333333333333</v>
       </c>
       <c r="M46" t="n">
-        <v>76431.09892175579</v>
+        <v>81460.76558842247</v>
       </c>
       <c r="N46" t="n">
-        <v>89918</v>
+        <v>100243</v>
       </c>
       <c r="O46" t="n">
-        <v>1397.666666666667</v>
+        <v>1557.666666666667</v>
       </c>
       <c r="P46" t="n">
-        <v>18875.60664431599</v>
+        <v>19158.77331098266</v>
       </c>
       <c r="Q46" t="n">
-        <v>54861</v>
+        <v>64613</v>
       </c>
       <c r="R46" t="n">
-        <v>759.3333333333334</v>
+        <v>830.3333333333334</v>
       </c>
       <c r="S46" t="n">
-        <v>31458.59305470858</v>
+        <v>32561.42638804191</v>
       </c>
       <c r="T46" t="n">
-        <v>44328</v>
+        <v>51968</v>
       </c>
       <c r="U46" t="n">
-        <v>1033.666666666667</v>
+        <v>1158</v>
       </c>
       <c r="V46" t="n">
-        <v>49511.11296941019</v>
+        <v>55076.77963607686</v>
       </c>
       <c r="W46" t="n">
-        <v>38867</v>
+        <v>47936</v>
       </c>
       <c r="X46" t="n">
-        <v>1258</v>
+        <v>1500.333333333333</v>
       </c>
       <c r="Y46" t="n">
-        <v>31458.59305470858</v>
+        <v>32561.42638804191</v>
       </c>
       <c r="Z46" t="n">
-        <v>44328</v>
+        <v>51968</v>
       </c>
       <c r="AA46" t="n">
-        <v>1033.666666666667</v>
+        <v>1158</v>
       </c>
       <c r="AB46" t="n">
-        <v>31458.59305470858</v>
+        <v>32561.42638804191</v>
       </c>
       <c r="AC46" t="n">
-        <v>44328</v>
+        <v>51968</v>
       </c>
       <c r="AD46" t="n">
-        <v>1033.666666666667</v>
+        <v>1158</v>
       </c>
       <c r="AE46" t="n">
-        <v>62775.81589069685</v>
+        <v>69521.81589069685</v>
       </c>
       <c r="AF46" t="n">
-        <v>47740</v>
+        <v>57211</v>
       </c>
       <c r="AG46" t="n">
-        <v>1512</v>
+        <v>1749</v>
       </c>
       <c r="AH46" t="n">
-        <v>46850.57593905871</v>
+        <v>52290.74260572538</v>
       </c>
       <c r="AI46" t="n">
-        <v>53619</v>
+        <v>62922</v>
       </c>
       <c r="AJ46" t="n">
-        <v>1295.333333333333</v>
+        <v>1537</v>
       </c>
       <c r="AK46" t="n">
-        <v>31458.59305470858</v>
+        <v>32561.42638804191</v>
       </c>
       <c r="AL46" t="n">
-        <v>44328</v>
+        <v>51968</v>
       </c>
       <c r="AM46" t="n">
-        <v>1033.666666666667</v>
+        <v>1158</v>
       </c>
       <c r="AN46" t="n">
-        <v>59583.21876488367</v>
+        <v>65522.05209821701</v>
       </c>
       <c r="AO46" t="n">
-        <v>45407</v>
+        <v>55224</v>
       </c>
       <c r="AP46" t="n">
-        <v>1465</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="47">
@@ -22529,115 +22529,115 @@
         <v>2</v>
       </c>
       <c r="F55" t="n">
-        <v>5837</v>
+        <v>6634</v>
       </c>
       <c r="G55" t="n">
-        <v>336677.9617338286</v>
+        <v>385034.9807979534</v>
       </c>
       <c r="H55" t="n">
-        <v>15608.35807168063</v>
+        <v>33138.5140508834</v>
       </c>
       <c r="I55" t="n">
-        <v>108488.1063041736</v>
+        <v>128077.3610702048</v>
       </c>
       <c r="J55" t="n">
-        <v>71120.55292203689</v>
+        <v>74525.92553902129</v>
       </c>
       <c r="K55" t="n">
-        <v>84995</v>
+        <v>106268</v>
       </c>
       <c r="L55" t="n">
-        <v>1409.666666666667</v>
+        <v>1581</v>
       </c>
       <c r="M55" t="n">
-        <v>77928.82503126655</v>
+        <v>83485.32416471542</v>
       </c>
       <c r="N55" t="n">
-        <v>89907</v>
+        <v>99536</v>
       </c>
       <c r="O55" t="n">
-        <v>1409.666666666667</v>
+        <v>1581</v>
       </c>
       <c r="P55" t="n">
-        <v>20911.65704288433</v>
+        <v>21834.88061307497</v>
       </c>
       <c r="Q55" t="n">
-        <v>54185</v>
+        <v>64515</v>
       </c>
       <c r="R55" t="n">
-        <v>791.3333333333334</v>
+        <v>877.6666666666667</v>
       </c>
       <c r="S55" t="n">
-        <v>34384.6965285475</v>
+        <v>35686.77625125114</v>
       </c>
       <c r="T55" t="n">
-        <v>42435</v>
+        <v>50035</v>
       </c>
       <c r="U55" t="n">
-        <v>1070</v>
+        <v>1201.333333333333</v>
       </c>
       <c r="V55" t="n">
-        <v>47420.06131603325</v>
+        <v>52712.2623558946</v>
       </c>
       <c r="W55" t="n">
-        <v>38807</v>
+        <v>48219</v>
       </c>
       <c r="X55" t="n">
-        <v>1224</v>
+        <v>1452</v>
       </c>
       <c r="Y55" t="n">
-        <v>34384.6965285475</v>
+        <v>35686.77625125114</v>
       </c>
       <c r="Z55" t="n">
-        <v>42435</v>
+        <v>50035</v>
       </c>
       <c r="AA55" t="n">
-        <v>1070</v>
+        <v>1201.333333333333</v>
       </c>
       <c r="AB55" t="n">
-        <v>34384.6965285475</v>
+        <v>35686.77625125114</v>
       </c>
       <c r="AC55" t="n">
-        <v>42435</v>
+        <v>50035</v>
       </c>
       <c r="AD55" t="n">
-        <v>1070</v>
+        <v>1201.333333333333</v>
       </c>
       <c r="AE55" t="n">
-        <v>65336.04276826824</v>
+        <v>71903.46044591122</v>
       </c>
       <c r="AF55" t="n">
-        <v>44986</v>
+        <v>54709</v>
       </c>
       <c r="AG55" t="n">
-        <v>1456.666666666667</v>
+        <v>1700.666666666667</v>
       </c>
       <c r="AH55" t="n">
-        <v>43768.95712474304</v>
+        <v>48886.46145749868</v>
       </c>
       <c r="AI55" t="n">
-        <v>52749</v>
+        <v>62357</v>
       </c>
       <c r="AJ55" t="n">
-        <v>1257.666666666667</v>
+        <v>1483</v>
       </c>
       <c r="AK55" t="n">
-        <v>34384.6965285475</v>
+        <v>35686.77625125114</v>
       </c>
       <c r="AL55" t="n">
-        <v>42435</v>
+        <v>50035</v>
       </c>
       <c r="AM55" t="n">
-        <v>1070</v>
+        <v>1201.333333333333</v>
       </c>
       <c r="AN55" t="n">
-        <v>61989.46092439249</v>
+        <v>68320.13683427118</v>
       </c>
       <c r="AO55" t="n">
-        <v>43876</v>
+        <v>53932</v>
       </c>
       <c r="AP55" t="n">
-        <v>1527</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="56">
@@ -23717,115 +23717,115 @@
         <v>2</v>
       </c>
       <c r="F64" t="n">
-        <v>5868</v>
+        <v>6666</v>
       </c>
       <c r="G64" t="n">
-        <v>338915.7934488271</v>
+        <v>387229.8728712098</v>
       </c>
       <c r="H64" t="n">
-        <v>39320.03873666607</v>
+        <v>52080.32754533034</v>
       </c>
       <c r="I64" t="n">
-        <v>114560.9877347062</v>
+        <v>134274.3451354282</v>
       </c>
       <c r="J64" t="n">
-        <v>70912.10956150132</v>
+        <v>74468.78826186233</v>
       </c>
       <c r="K64" t="n">
-        <v>88917</v>
+        <v>110866</v>
       </c>
       <c r="L64" t="n">
-        <v>1411.666666666667</v>
+        <v>1584.666666666667</v>
       </c>
       <c r="M64" t="n">
-        <v>78100.92879777547</v>
+        <v>83990.45948369605</v>
       </c>
       <c r="N64" t="n">
-        <v>88911</v>
+        <v>98743</v>
       </c>
       <c r="O64" t="n">
-        <v>1411.666666666667</v>
+        <v>1584.666666666667</v>
       </c>
       <c r="P64" t="n">
-        <v>21965.14231780776</v>
+        <v>22879.04123477526</v>
       </c>
       <c r="Q64" t="n">
-        <v>55184</v>
+        <v>65456</v>
       </c>
       <c r="R64" t="n">
-        <v>807.3333333333334</v>
+        <v>890.6666666666667</v>
       </c>
       <c r="S64" t="n">
-        <v>33766.11074023078</v>
+        <v>35172.78944059178</v>
       </c>
       <c r="T64" t="n">
-        <v>41632</v>
+        <v>49111</v>
       </c>
       <c r="U64" t="n">
-        <v>1081</v>
+        <v>1217.666666666667</v>
       </c>
       <c r="V64" t="n">
-        <v>46875.54359043517</v>
+        <v>52187.63745325105</v>
       </c>
       <c r="W64" t="n">
-        <v>39069</v>
+        <v>48484</v>
       </c>
       <c r="X64" t="n">
-        <v>1224</v>
+        <v>1448</v>
       </c>
       <c r="Y64" t="n">
-        <v>33766.11074023078</v>
+        <v>35172.78944059178</v>
       </c>
       <c r="Z64" t="n">
-        <v>41632</v>
+        <v>49111</v>
       </c>
       <c r="AA64" t="n">
-        <v>1081</v>
+        <v>1217.666666666667</v>
       </c>
       <c r="AB64" t="n">
-        <v>33766.11074023078</v>
+        <v>35172.78944059178</v>
       </c>
       <c r="AC64" t="n">
-        <v>41632</v>
+        <v>49111</v>
       </c>
       <c r="AD64" t="n">
-        <v>1081</v>
+        <v>1217.666666666667</v>
       </c>
       <c r="AE64" t="n">
-        <v>65389.35818269619</v>
+        <v>72577.08381446514</v>
       </c>
       <c r="AF64" t="n">
-        <v>47129</v>
+        <v>56970</v>
       </c>
       <c r="AG64" t="n">
-        <v>1443.666666666667</v>
+        <v>1682.666666666667</v>
       </c>
       <c r="AH64" t="n">
-        <v>44333.00797596798</v>
+        <v>49596.18487127484</v>
       </c>
       <c r="AI64" t="n">
-        <v>54515</v>
+        <v>64063</v>
       </c>
       <c r="AJ64" t="n">
-        <v>1262</v>
+        <v>1485.666666666667</v>
       </c>
       <c r="AK64" t="n">
-        <v>33766.11074023078</v>
+        <v>35172.78944059178</v>
       </c>
       <c r="AL64" t="n">
-        <v>41632</v>
+        <v>49111</v>
       </c>
       <c r="AM64" t="n">
-        <v>1081</v>
+        <v>1217.666666666667</v>
       </c>
       <c r="AN64" t="n">
-        <v>62553.73905247665</v>
+        <v>69310.77876366799</v>
       </c>
       <c r="AO64" t="n">
-        <v>44544</v>
+        <v>54643</v>
       </c>
       <c r="AP64" t="n">
-        <v>1547.333333333333</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="65">
@@ -24905,115 +24905,115 @@
         <v>2</v>
       </c>
       <c r="F73" t="n">
-        <v>5743</v>
+        <v>6558</v>
       </c>
       <c r="G73" t="n">
-        <v>330894.1964498445</v>
+        <v>380606.6258283756</v>
       </c>
       <c r="H73" t="n">
-        <v>55065.5539454457</v>
+        <v>75188.34113941934</v>
       </c>
       <c r="I73" t="n">
-        <v>131240.5877564872</v>
+        <v>152576.1809768262</v>
       </c>
       <c r="J73" t="n">
-        <v>76361.1759073932</v>
+        <v>80152.32468328775</v>
       </c>
       <c r="K73" t="n">
-        <v>91572</v>
+        <v>114761</v>
       </c>
       <c r="L73" t="n">
-        <v>1432</v>
+        <v>1607.333333333333</v>
       </c>
       <c r="M73" t="n">
-        <v>84168.70168839947</v>
+        <v>90172.84481457649</v>
       </c>
       <c r="N73" t="n">
-        <v>87851</v>
+        <v>97463</v>
       </c>
       <c r="O73" t="n">
-        <v>1432</v>
+        <v>1607.333333333333</v>
       </c>
       <c r="P73" t="n">
-        <v>27228.28557032703</v>
+        <v>28137.89009010103</v>
       </c>
       <c r="Q73" t="n">
-        <v>53865</v>
+        <v>64329</v>
       </c>
       <c r="R73" t="n">
-        <v>782.6666666666666</v>
+        <v>869.6666666666666</v>
       </c>
       <c r="S73" t="n">
-        <v>36676.84709509888</v>
+        <v>37960.08626647364</v>
       </c>
       <c r="T73" t="n">
-        <v>41022</v>
+        <v>47898</v>
       </c>
       <c r="U73" t="n">
-        <v>1053.666666666667</v>
+        <v>1195.666666666667</v>
       </c>
       <c r="V73" t="n">
-        <v>51952.71071264434</v>
+        <v>57129.73519475357</v>
       </c>
       <c r="W73" t="n">
-        <v>39321</v>
+        <v>48963</v>
       </c>
       <c r="X73" t="n">
-        <v>1216.333333333333</v>
+        <v>1445.666666666667</v>
       </c>
       <c r="Y73" t="n">
-        <v>36676.84709509888</v>
+        <v>37960.08626647364</v>
       </c>
       <c r="Z73" t="n">
-        <v>41022</v>
+        <v>47898</v>
       </c>
       <c r="AA73" t="n">
-        <v>1053.666666666667</v>
+        <v>1195.666666666667</v>
       </c>
       <c r="AB73" t="n">
-        <v>36676.84709509888</v>
+        <v>37960.08626647364</v>
       </c>
       <c r="AC73" t="n">
-        <v>41022</v>
+        <v>47898</v>
       </c>
       <c r="AD73" t="n">
-        <v>1053.666666666667</v>
+        <v>1195.666666666667</v>
       </c>
       <c r="AE73" t="n">
-        <v>73772.43042552058</v>
+        <v>81002.1856044283</v>
       </c>
       <c r="AF73" t="n">
-        <v>49998</v>
+        <v>60205</v>
       </c>
       <c r="AG73" t="n">
-        <v>1522.333333333333</v>
+        <v>1767.666666666667</v>
       </c>
       <c r="AH73" t="n">
-        <v>49242.09440054239</v>
+        <v>54405.37123670058</v>
       </c>
       <c r="AI73" t="n">
-        <v>51905</v>
+        <v>61623</v>
       </c>
       <c r="AJ73" t="n">
-        <v>1259.333333333333</v>
+        <v>1490</v>
       </c>
       <c r="AK73" t="n">
-        <v>36676.84709509888</v>
+        <v>37960.08626647364</v>
       </c>
       <c r="AL73" t="n">
-        <v>41022</v>
+        <v>47898</v>
       </c>
       <c r="AM73" t="n">
-        <v>1053.666666666667</v>
+        <v>1195.666666666667</v>
       </c>
       <c r="AN73" t="n">
-        <v>69780.63237262685</v>
+        <v>76890.99018806941</v>
       </c>
       <c r="AO73" t="n">
-        <v>47745</v>
+        <v>57926</v>
       </c>
       <c r="AP73" t="n">
-        <v>1511.333333333333</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="74">
@@ -26093,115 +26093,115 @@
         <v>2</v>
       </c>
       <c r="F82" t="n">
-        <v>5757</v>
+        <v>6596</v>
       </c>
       <c r="G82" t="n">
-        <v>331572.6103415878</v>
+        <v>383211.5867195405</v>
       </c>
       <c r="H82" t="n">
-        <v>98360.91701888156</v>
+        <v>118565.4445779367</v>
       </c>
       <c r="I82" t="n">
-        <v>123713.9895987293</v>
+        <v>146627.7691262884</v>
       </c>
       <c r="J82" t="n">
-        <v>75912.02543689795</v>
+        <v>80524.82071248851</v>
       </c>
       <c r="K82" t="n">
-        <v>93967</v>
+        <v>117133</v>
       </c>
       <c r="L82" t="n">
-        <v>1428</v>
+        <v>1614</v>
       </c>
       <c r="M82" t="n">
-        <v>83235.05214430622</v>
+        <v>90566.74505769204</v>
       </c>
       <c r="N82" t="n">
-        <v>89014</v>
+        <v>98606</v>
       </c>
       <c r="O82" t="n">
-        <v>1428</v>
+        <v>1614</v>
       </c>
       <c r="P82" t="n">
-        <v>29830.83902832562</v>
+        <v>30828.87052438861</v>
       </c>
       <c r="Q82" t="n">
-        <v>53500</v>
+        <v>64220</v>
       </c>
       <c r="R82" t="n">
-        <v>831.9999999999999</v>
+        <v>920.6666666666665</v>
       </c>
       <c r="S82" t="n">
-        <v>37356.64638626782</v>
+        <v>38951.7251264253</v>
       </c>
       <c r="T82" t="n">
-        <v>40220</v>
+        <v>46812</v>
       </c>
       <c r="U82" t="n">
-        <v>1072.666666666667</v>
+        <v>1222.666666666667</v>
       </c>
       <c r="V82" t="n">
-        <v>53666.28866647162</v>
+        <v>57601.91858773147</v>
       </c>
       <c r="W82" t="n">
-        <v>40913</v>
+        <v>52372</v>
       </c>
       <c r="X82" t="n">
-        <v>1249.333333333333</v>
+        <v>1444.333333333333</v>
       </c>
       <c r="Y82" t="n">
-        <v>37356.64638626782</v>
+        <v>38951.7251264253</v>
       </c>
       <c r="Z82" t="n">
-        <v>40220</v>
+        <v>46812</v>
       </c>
       <c r="AA82" t="n">
-        <v>1072.666666666667</v>
+        <v>1222.666666666667</v>
       </c>
       <c r="AB82" t="n">
-        <v>37356.64638626782</v>
+        <v>38951.7251264253</v>
       </c>
       <c r="AC82" t="n">
-        <v>40220</v>
+        <v>46812</v>
       </c>
       <c r="AD82" t="n">
-        <v>1072.666666666667</v>
+        <v>1222.666666666667</v>
       </c>
       <c r="AE82" t="n">
-        <v>71263.64838323693</v>
+        <v>76292.97909189835</v>
       </c>
       <c r="AF82" t="n">
-        <v>51506</v>
+        <v>63259</v>
       </c>
       <c r="AG82" t="n">
-        <v>1536.666666666667</v>
+        <v>1740</v>
       </c>
       <c r="AH82" t="n">
-        <v>50675.42133641148</v>
+        <v>54592.94102145085</v>
       </c>
       <c r="AI82" t="n">
-        <v>51838</v>
+        <v>63323</v>
       </c>
       <c r="AJ82" t="n">
-        <v>1270</v>
+        <v>1463.666666666667</v>
       </c>
       <c r="AK82" t="n">
-        <v>37356.64638626782</v>
+        <v>38951.7251264253</v>
       </c>
       <c r="AL82" t="n">
-        <v>40220</v>
+        <v>46812</v>
       </c>
       <c r="AM82" t="n">
-        <v>1072.666666666667</v>
+        <v>1222.666666666667</v>
       </c>
       <c r="AN82" t="n">
-        <v>69354.96610357317</v>
+        <v>73818.15507995112</v>
       </c>
       <c r="AO82" t="n">
-        <v>53384</v>
+        <v>65484</v>
       </c>
       <c r="AP82" t="n">
-        <v>1544.333333333333</v>
+        <v>1750.333333333333</v>
       </c>
     </row>
     <row r="83">
@@ -27281,115 +27281,115 @@
         <v>2</v>
       </c>
       <c r="F91" t="n">
-        <v>5836</v>
+        <v>6651</v>
       </c>
       <c r="G91" t="n">
-        <v>337133.5547279215</v>
+        <v>386821.3897794679</v>
       </c>
       <c r="H91" t="n">
-        <v>87369.33929781331</v>
+        <v>106074.2877514216</v>
       </c>
       <c r="I91" t="n">
-        <v>136021.43593398</v>
+        <v>157692.3637690315</v>
       </c>
       <c r="J91" t="n">
-        <v>83737.56526910239</v>
+        <v>87260.45186704054</v>
       </c>
       <c r="K91" t="n">
-        <v>95551</v>
+        <v>117151</v>
       </c>
       <c r="L91" t="n">
-        <v>1535</v>
+        <v>1699.666666666667</v>
       </c>
       <c r="M91" t="n">
-        <v>91288.7766445373</v>
+        <v>96997.02406721772</v>
       </c>
       <c r="N91" t="n">
-        <v>84707</v>
+        <v>93814</v>
       </c>
       <c r="O91" t="n">
-        <v>1535</v>
+        <v>1699.666666666667</v>
       </c>
       <c r="P91" t="n">
-        <v>36173.19540339302</v>
+        <v>36932.57684669199</v>
       </c>
       <c r="Q91" t="n">
-        <v>54415</v>
+        <v>65021</v>
       </c>
       <c r="R91" t="n">
-        <v>890</v>
+        <v>970.3333333333334</v>
       </c>
       <c r="S91" t="n">
-        <v>37930.45893448552</v>
+        <v>39406.95377984634</v>
       </c>
       <c r="T91" t="n">
-        <v>39628</v>
+        <v>45719</v>
       </c>
       <c r="U91" t="n">
-        <v>1126.333333333333</v>
+        <v>1270.333333333333</v>
       </c>
       <c r="V91" t="n">
-        <v>53638.91978378115</v>
+        <v>58396.23937141002</v>
       </c>
       <c r="W91" t="n">
-        <v>47556</v>
+        <v>59276</v>
       </c>
       <c r="X91" t="n">
-        <v>1265.333333333333</v>
+        <v>1471.333333333333</v>
       </c>
       <c r="Y91" t="n">
-        <v>37930.45893448552</v>
+        <v>39406.95377984634</v>
       </c>
       <c r="Z91" t="n">
-        <v>39628</v>
+        <v>45719</v>
       </c>
       <c r="AA91" t="n">
-        <v>1126.333333333333</v>
+        <v>1270.333333333333</v>
       </c>
       <c r="AB91" t="n">
-        <v>37930.45893448552</v>
+        <v>39406.95377984634</v>
       </c>
       <c r="AC91" t="n">
-        <v>39628</v>
+        <v>45719</v>
       </c>
       <c r="AD91" t="n">
-        <v>1126.333333333333</v>
+        <v>1270.333333333333</v>
       </c>
       <c r="AE91" t="n">
-        <v>62366.34153641525</v>
+        <v>66877.2693714668</v>
       </c>
       <c r="AF91" t="n">
-        <v>60165</v>
+        <v>71530</v>
       </c>
       <c r="AG91" t="n">
-        <v>1520.333333333333</v>
+        <v>1707.666666666667</v>
       </c>
       <c r="AH91" t="n">
-        <v>51046.22589198168</v>
+        <v>55835.09187136313</v>
       </c>
       <c r="AI91" t="n">
-        <v>64714</v>
+        <v>76488</v>
       </c>
       <c r="AJ91" t="n">
-        <v>1250.333333333333</v>
+        <v>1456</v>
       </c>
       <c r="AK91" t="n">
-        <v>37930.45893448552</v>
+        <v>39406.95377984634</v>
       </c>
       <c r="AL91" t="n">
-        <v>39628</v>
+        <v>45719</v>
       </c>
       <c r="AM91" t="n">
-        <v>1126.333333333333</v>
+        <v>1270.333333333333</v>
       </c>
       <c r="AN91" t="n">
-        <v>60126.16159275653</v>
+        <v>64642.45025255034</v>
       </c>
       <c r="AO91" t="n">
-        <v>59246</v>
+        <v>70868</v>
       </c>
       <c r="AP91" t="n">
-        <v>1578.666666666667</v>
+        <v>1779.666666666667</v>
       </c>
     </row>
     <row r="92">
@@ -28469,115 +28469,115 @@
         <v>2</v>
       </c>
       <c r="F100" t="n">
-        <v>5858</v>
+        <v>6702</v>
       </c>
       <c r="G100" t="n">
-        <v>339679.0664673753</v>
+        <v>391885.7764240853</v>
       </c>
       <c r="H100" t="n">
-        <v>83497.6408835763</v>
+        <v>98884.00451993993</v>
       </c>
       <c r="I100" t="n">
-        <v>127771.5528987114</v>
+        <v>149873.284500443</v>
       </c>
       <c r="J100" t="n">
-        <v>81776.17370342468</v>
+        <v>86075.09145234243</v>
       </c>
       <c r="K100" t="n">
-        <v>95081</v>
+        <v>117263</v>
       </c>
       <c r="L100" t="n">
-        <v>1522.666666666667</v>
+        <v>1696</v>
       </c>
       <c r="M100" t="n">
-        <v>89485.65505501024</v>
+        <v>96339.55115890634</v>
       </c>
       <c r="N100" t="n">
-        <v>87353</v>
+        <v>96862</v>
       </c>
       <c r="O100" t="n">
-        <v>1522.666666666667</v>
+        <v>1696</v>
       </c>
       <c r="P100" t="n">
-        <v>35982.87702205896</v>
+        <v>36836.12377530572</v>
       </c>
       <c r="Q100" t="n">
-        <v>54646</v>
+        <v>65729</v>
       </c>
       <c r="R100" t="n">
-        <v>889</v>
+        <v>976</v>
       </c>
       <c r="S100" t="n">
-        <v>37826.78447471155</v>
+        <v>39507.30395523104</v>
       </c>
       <c r="T100" t="n">
-        <v>39579</v>
+        <v>45844</v>
       </c>
       <c r="U100" t="n">
-        <v>1118</v>
+        <v>1273</v>
       </c>
       <c r="V100" t="n">
-        <v>52273.157209377</v>
+        <v>54917.74595396574</v>
       </c>
       <c r="W100" t="n">
-        <v>47249</v>
+        <v>60235</v>
       </c>
       <c r="X100" t="n">
-        <v>1265.333333333333</v>
+        <v>1426.666666666667</v>
       </c>
       <c r="Y100" t="n">
-        <v>37826.78447471155</v>
+        <v>39507.30395523104</v>
       </c>
       <c r="Z100" t="n">
-        <v>39579</v>
+        <v>45844</v>
       </c>
       <c r="AA100" t="n">
-        <v>1118.333333333333</v>
+        <v>1273.333333333333</v>
       </c>
       <c r="AB100" t="n">
-        <v>37826.78447471155</v>
+        <v>39507.30395523104</v>
       </c>
       <c r="AC100" t="n">
-        <v>39579</v>
+        <v>45844</v>
       </c>
       <c r="AD100" t="n">
-        <v>1118</v>
+        <v>1273</v>
       </c>
       <c r="AE100" t="n">
-        <v>60882.98942840926</v>
+        <v>64578.4439738638</v>
       </c>
       <c r="AF100" t="n">
-        <v>59080</v>
+        <v>70591</v>
       </c>
       <c r="AG100" t="n">
-        <v>1527</v>
+        <v>1692.333333333333</v>
       </c>
       <c r="AH100" t="n">
-        <v>49905.37699511323</v>
+        <v>52750.83154056778</v>
       </c>
       <c r="AI100" t="n">
-        <v>64757</v>
+        <v>77770</v>
       </c>
       <c r="AJ100" t="n">
-        <v>1247.333333333333</v>
+        <v>1412</v>
       </c>
       <c r="AK100" t="n">
-        <v>37826.78447471155</v>
+        <v>39507.30395523104</v>
       </c>
       <c r="AL100" t="n">
-        <v>39579</v>
+        <v>45844</v>
       </c>
       <c r="AM100" t="n">
-        <v>1118</v>
+        <v>1273</v>
       </c>
       <c r="AN100" t="n">
-        <v>59058.92317024834</v>
+        <v>63685.54654687172</v>
       </c>
       <c r="AO100" t="n">
-        <v>61558</v>
+        <v>73737</v>
       </c>
       <c r="AP100" t="n">
-        <v>1603.333333333333</v>
+        <v>1802.333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>